<commit_message>
Zarca NS reading done
</commit_message>
<xml_diff>
--- a/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_Performance.xlsx
+++ b/Engage/Engage-Performance/src/main/resources/excelfiles/Engage_Performance.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0130E14-ED78-42E4-9816-8495ACEA66F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="1" r:id="rId1"/>
@@ -12,7 +13,7 @@
     <sheet name="Users" sheetId="2" r:id="rId3"/>
     <sheet name="PerformanceTC" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>Environment</t>
   </si>
@@ -69,9 +70,6 @@
     <t>Owner</t>
   </si>
   <si>
-    <t>Sanket</t>
-  </si>
-  <si>
     <t>Test_Name</t>
   </si>
   <si>
@@ -96,9 +94,6 @@
     <t>Expected3</t>
   </si>
   <si>
-    <t>https://www.sogosurvey.com/</t>
-  </si>
-  <si>
     <t>Performance_TC1</t>
   </si>
   <si>
@@ -108,12 +103,6 @@
     <t>TimeLoad</t>
   </si>
   <si>
-    <t>SoGo@NS3196</t>
-  </si>
-  <si>
-    <t>sogo_jk_enterprise</t>
-  </si>
-  <si>
     <t>Platform Log in</t>
   </si>
   <si>
@@ -123,17 +112,164 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>9.32</t>
-  </si>
-  <si>
     <t>Engage Platform</t>
+  </si>
+  <si>
+    <t>sharlot_test</t>
+  </si>
+  <si>
+    <t>Zarca@NS3196</t>
+  </si>
+  <si>
+    <t>https://research.zarca.com/static/REGISTER/ClientLogin.aspx</t>
+  </si>
+  <si>
+    <t>Performance_TC2</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>Load SM Tab</t>
+  </si>
+  <si>
+    <t>Capture the page load time of SM Tab</t>
+  </si>
+  <si>
+    <t>Note page load time</t>
+  </si>
+  <si>
+    <t>Night Support Readings,2078</t>
+  </si>
+  <si>
+    <t>Performance_TC3</t>
+  </si>
+  <si>
+    <t>Depositing a Question in QB</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Depositing in Question Bank</t>
+  </si>
+  <si>
+    <t>Performance_TC4</t>
+  </si>
+  <si>
+    <t>Add Comment</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Add Comment</t>
+  </si>
+  <si>
+    <t>Night Support Readings,2078,Additional suggestions do you have for improving the support for new teachers at this school</t>
+  </si>
+  <si>
+    <t>Performance_TC5</t>
+  </si>
+  <si>
+    <t>Delete Comment</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Delete Comment</t>
+  </si>
+  <si>
+    <t>Performance_TC6</t>
+  </si>
+  <si>
+    <t>Move Page</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Move Page</t>
+  </si>
+  <si>
+    <t>Night Support Readings,2078,1</t>
+  </si>
+  <si>
+    <t>Performance_TC7</t>
+  </si>
+  <si>
+    <t>Move Matrix Grid</t>
+  </si>
+  <si>
+    <t>Capture the page load time of moving Matrix Grid question</t>
+  </si>
+  <si>
+    <t>Performance_TC8</t>
+  </si>
+  <si>
+    <t>Load DM Tab</t>
+  </si>
+  <si>
+    <t>Capture the page load time of DM Tab</t>
+  </si>
+  <si>
+    <t>Performance_TC9</t>
+  </si>
+  <si>
+    <t>Load RM tab</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Report Tab</t>
+  </si>
+  <si>
+    <t>Survey # 201 RMX NS Reading,201</t>
+  </si>
+  <si>
+    <t>Performance_TC10</t>
+  </si>
+  <si>
+    <t>Load OMNI Report</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Omni Report</t>
+  </si>
+  <si>
+    <t>Performance_TC11</t>
+  </si>
+  <si>
+    <t>Logout</t>
+  </si>
+  <si>
+    <t>Capture the page load time of Logout</t>
+  </si>
+  <si>
+    <t>7.92</t>
+  </si>
+  <si>
+    <t>11.26</t>
+  </si>
+  <si>
+    <t>5.55</t>
+  </si>
+  <si>
+    <t>5.24</t>
+  </si>
+  <si>
+    <t>9.51</t>
+  </si>
+  <si>
+    <t>4.58</t>
+  </si>
+  <si>
+    <t>8.04</t>
+  </si>
+  <si>
+    <t>13.72</t>
+  </si>
+  <si>
+    <t>3.28</t>
+  </si>
+  <si>
+    <t>2.38</t>
+  </si>
+  <si>
+    <t>9.35</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -167,6 +303,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -226,14 +369,14 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -248,10 +391,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -532,12 +675,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,19 +705,22 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{7C606FED-5AEC-4CC5-85C8-17130D54BD9E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -604,7 +750,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -616,12 +762,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,10 +797,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>3</v>
@@ -667,12 +813,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,42 +855,42 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>18</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -753,34 +899,466 @@
         <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="5"/>
+      <c r="I2" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="J2" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="6"/>
       <c r="M2" s="4"/>
       <c r="N2" s="1"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="L3" s="6"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="L4" s="6"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="L5" s="6"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="4"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="4"/>
+      <c r="P6" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="H3" r:id="rId1" xr:uid="{3E39C0E6-D5F3-4AFA-81CE-34E8539BE7BE}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{5654DFE0-2D67-4F65-9E82-1C8E8CEC884C}"/>
+    <hyperlink ref="H5" r:id="rId3" xr:uid="{94DE5C0F-AABE-438B-8413-80F89E6B6BDB}"/>
+    <hyperlink ref="H6" r:id="rId4" xr:uid="{B1DD290A-D0F5-4051-83AB-5D707014677B}"/>
+    <hyperlink ref="H7" r:id="rId5" xr:uid="{820CB4EC-A17F-40BB-AE02-33B50BD1C1ED}"/>
+    <hyperlink ref="H8" r:id="rId6" xr:uid="{1B6EE435-AC39-42F1-9C3F-93C4F7EAEE8C}"/>
+    <hyperlink ref="H9" r:id="rId7" xr:uid="{9727B971-82B2-4294-9EB4-FBC94C962566}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{961E4746-EE00-4240-A73E-FEDDB2F64F62}"/>
+    <hyperlink ref="H11" r:id="rId9" xr:uid="{21314E19-7065-4F5D-8545-2D06CD3B4720}"/>
+    <hyperlink ref="H12" r:id="rId10" xr:uid="{827CFC7D-AFA6-4ED5-B296-39C189A4A3E4}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>